<commit_message>
Change component to iron for water quality case study
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BFF46E-F655-4AC7-958E-AFD75318A040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707715DE-1584-42EE-8045-A6EA922E0031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="14" activeTab="35" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="55" activeTab="55" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -968,9 +968,6 @@
     <t>PADS</t>
   </si>
   <si>
-    <t>TDS</t>
-  </si>
-  <si>
     <t>Initial Water Quality at Storage (mg/L)</t>
   </si>
   <si>
@@ -981,6 +978,9 @@
   </si>
   <si>
     <t>Table of Node Capacity Capacity  [bbl/week] * absence of node or empty cell signifies no max capacity</t>
+  </si>
+  <si>
+    <t>Iron</t>
   </si>
 </sst>
 </file>
@@ -12178,7 +12178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27E83FA-0F3B-443C-8B3E-ADC37406AEAD}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -12191,7 +12191,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -17166,8 +17166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17185,7 +17185,7 @@
         <v>255</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -25788,7 +25788,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="B18" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25812,7 +25812,7 @@
         <v>277</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25820,7 +25820,7 @@
         <v>130</v>
       </c>
       <c r="B3" s="73">
-        <v>142277</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25828,7 +25828,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="74">
-        <v>140998</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25836,7 +25836,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="74">
-        <v>172490.2</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25844,7 +25844,7 @@
         <v>122</v>
       </c>
       <c r="B6" s="74">
-        <v>257547</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25852,7 +25852,7 @@
         <v>123</v>
       </c>
       <c r="B7" s="74">
-        <v>241833.8</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25860,7 +25860,7 @@
         <v>124</v>
       </c>
       <c r="B8" s="74">
-        <v>188503.7</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25868,7 +25868,7 @@
         <v>125</v>
       </c>
       <c r="B9" s="74">
-        <v>146716</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25876,7 +25876,7 @@
         <v>126</v>
       </c>
       <c r="B10" s="74">
-        <v>216563</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25884,7 +25884,7 @@
         <v>127</v>
       </c>
       <c r="B11" s="74">
-        <v>150626</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25892,7 +25892,7 @@
         <v>128</v>
       </c>
       <c r="B12" s="74">
-        <v>247061</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25900,7 +25900,7 @@
         <v>129</v>
       </c>
       <c r="B13" s="74">
-        <v>180968</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25908,7 +25908,7 @@
         <v>131</v>
       </c>
       <c r="B14" s="74">
-        <v>195584</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25916,7 +25916,7 @@
         <v>132</v>
       </c>
       <c r="B15" s="74">
-        <v>148655</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25924,7 +25924,7 @@
         <v>133</v>
       </c>
       <c r="B16" s="74">
-        <v>185369</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25932,7 +25932,7 @@
         <v>134</v>
       </c>
       <c r="B17" s="74">
-        <v>222724</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25940,7 +25940,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="74">
-        <v>165376</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25948,7 +25948,7 @@
         <v>135</v>
       </c>
       <c r="B19" s="74">
-        <v>240977</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -25956,7 +25956,7 @@
         <v>136</v>
       </c>
       <c r="B20" s="74">
-        <v>192794</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25964,7 +25964,7 @@
         <v>137</v>
       </c>
       <c r="B21" s="75">
-        <v>216769</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -25978,7 +25978,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25988,15 +25988,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26004,7 +26004,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="77">
-        <v>150000</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -26017,7 +26017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BFA9F4-87E5-4A8C-BA81-50B58EA7DF44}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26026,7 +26028,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -26034,7 +26036,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -26042,7 +26044,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="74">
-        <v>150000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -26050,7 +26052,7 @@
         <v>135</v>
       </c>
       <c r="B4" s="74">
-        <v>150000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -26058,7 +26060,7 @@
         <v>136</v>
       </c>
       <c r="B5" s="74">
-        <v>150000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26066,7 +26068,7 @@
         <v>137</v>
       </c>
       <c r="B6" s="75">
-        <v>150000</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>